<commit_message>
Updated keywords for fgDeGender
</commit_message>
<xml_diff>
--- a/Photo Club Hub/Documentation/fgDeGender_Trefwoorden.xlsx
+++ b/Photo Club Hub/Documentation/fgDeGender_Trefwoorden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Developer/XCode13Projects/SwiftUI/Photo Club Hub/Photo Club Hub/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986D8F6E-C661-C942-87DD-1EF27F8556E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1807C898-FAB2-2549-A2C6-E0D805D1D52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26440" xr2:uid="{186BA102-7DEB-D04F-9935-E140A076FA03}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="71">
   <si>
     <t>Albert</t>
   </si>
@@ -416,6 +416,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -424,9 +427,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1603,7 +1603,7 @@
   <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AA21" sqref="AA21"/>
+      <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
@@ -1625,65 +1625,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
       <c r="T1" s="19">
         <v>45774</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22" t="s">
+      <c r="A2" s="22"/>
+      <c r="B2" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="21"/>
-      <c r="B3" s="22" t="s">
+      <c r="A3" s="22"/>
+      <c r="B3" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
-      <c r="B4" s="22" t="s">
+      <c r="A4" s="22"/>
+      <c r="B4" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
     </row>
     <row r="6" spans="1:20" s="2" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -1855,7 +1855,7 @@
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
-      <c r="H10" s="23" t="s">
+      <c r="H10" s="20" t="s">
         <v>15</v>
       </c>
       <c r="I10" s="10"/>
@@ -2477,8 +2477,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="65" x14ac:dyDescent="0.3">
-      <c r="A29" s="12"/>
+    <row r="29" spans="1:20" ht="39" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
+        <v>63</v>
+      </c>
       <c r="B29" s="13" t="s">
         <v>61</v>
       </c>
@@ -2490,16 +2492,18 @@
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
-      <c r="I29" s="9" t="s">
-        <v>2</v>
-      </c>
+      <c r="I29" s="9"/>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
+      <c r="O29" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="P29" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="Q29" s="9" t="s">
         <v>9</v>
       </c>
@@ -2508,7 +2512,7 @@
       <c r="T29" s="12">
         <f>COUNTA(Table1[[#This Row],[eventueel voorstel voor 
 nieuw trefwoord]:[Zwart-wit]])</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
@@ -2556,7 +2560,7 @@
       </c>
       <c r="I31" s="16">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J31" s="16">
         <f t="shared" si="0"/>
@@ -2580,11 +2584,11 @@
       </c>
       <c r="O31" s="16">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P31" s="16">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q31" s="16">
         <f t="shared" si="0"/>

</xml_diff>